<commit_message>
FIX SOME TYPO OF THEMES
</commit_message>
<xml_diff>
--- a/THEME.xlsx
+++ b/THEME.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Dropbox/2017 Fall/amicus brief/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Documents/Amicus-Brief/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="1120" windowWidth="19740" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="8200" yWindow="460" windowWidth="19740" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Interest-group-09-15" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="382">
   <si>
     <t>CASE-NAME</t>
   </si>
@@ -1079,7 +1079,97 @@
     <t>TERRORIST ACT</t>
   </si>
   <si>
-    <t>SECOND AMENDMENT</t>
+    <t>DISADVANTAGED</t>
+  </si>
+  <si>
+    <t>SMALL BUSINESS</t>
+  </si>
+  <si>
+    <t>PROTECTION</t>
+  </si>
+  <si>
+    <t>EQUAL PROTECTION</t>
+  </si>
+  <si>
+    <t>RECORD</t>
+  </si>
+  <si>
+    <t>ECONOMIC</t>
+  </si>
+  <si>
+    <t>SOCIAL</t>
+  </si>
+  <si>
+    <t>DELEGATION</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>MINORITY</t>
+  </si>
+  <si>
+    <t>PARTICIPATION</t>
+  </si>
+  <si>
+    <t>LGBT</t>
+  </si>
+  <si>
+    <t>POLITICAL RIGHTS</t>
+  </si>
+  <si>
+    <t>ENGLISH SPEAKING</t>
+  </si>
+  <si>
+    <t>STATE INTEREST</t>
+  </si>
+  <si>
+    <t>SERVICES</t>
+  </si>
+  <si>
+    <t>EFFICIENCY</t>
+  </si>
+  <si>
+    <t>COMMUNICATION</t>
+  </si>
+  <si>
+    <t>TARGETED RECRUITMENT</t>
+  </si>
+  <si>
+    <t>LEGISLATIVE HISTORY</t>
+  </si>
+  <si>
+    <t>SECURITY</t>
+  </si>
+  <si>
+    <t>LEGISLATIVE PURPOSE</t>
+  </si>
+  <si>
+    <t>VAGUE</t>
+  </si>
+  <si>
+    <t>ARBITRARY ENFORCEMENT</t>
+  </si>
+  <si>
+    <t>COMMUNITY POLICE SERVICE</t>
+  </si>
+  <si>
+    <t>POLICY PRACTICE</t>
+  </si>
+  <si>
+    <t>CENSUS</t>
+  </si>
+  <si>
+    <t>VOTING RIGHTS</t>
+  </si>
+  <si>
+    <t>EQUALITY</t>
+  </si>
+  <si>
+    <t>SEX ORIENTATION</t>
+  </si>
+  <si>
+    <t>PLURALISM</t>
   </si>
 </sst>
 </file>
@@ -1122,10 +1212,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1406,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H358"/>
+  <dimension ref="A1:H394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E288" sqref="E288"/>
+    <sheetView tabSelected="1" topLeftCell="A369" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F391" sqref="F391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6349,7 +6440,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>185</v>
       </c>
@@ -6362,6 +6453,9 @@
       <c r="D288" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F288" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="G288" s="1" t="s">
         <v>17</v>
       </c>
@@ -6369,7 +6463,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>185</v>
       </c>
@@ -6382,6 +6476,9 @@
       <c r="D289" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F289" s="3" t="s">
+        <v>324</v>
+      </c>
       <c r="G289" s="1" t="s">
         <v>10</v>
       </c>
@@ -6389,7 +6486,17 @@
         <v>186</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F290" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F291" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>185</v>
       </c>
@@ -6402,6 +6509,12 @@
       <c r="D292" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E292" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F292" s="3" t="s">
+        <v>230</v>
+      </c>
       <c r="G292" s="1" t="s">
         <v>17</v>
       </c>
@@ -6409,67 +6522,73 @@
         <v>187</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A295" s="1" t="s">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F293" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F294" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F295" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B295" s="2" t="s">
+      <c r="B296" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C295" s="1">
+      <c r="C296" s="1">
         <v>1994</v>
       </c>
-      <c r="D295" s="1" t="s">
+      <c r="D296" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G295" s="1" t="s">
+      <c r="E296" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F296" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G296" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H295" s="1" t="s">
+      <c r="H296" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A298" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B298" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C298" s="1">
-        <v>1994</v>
-      </c>
-      <c r="D298" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G298" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H298" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A301" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B301" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C301" s="1">
-        <v>1994</v>
-      </c>
-      <c r="D301" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G301" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H301" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F297" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F298" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F299" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F300" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F301" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>185</v>
       </c>
@@ -6480,330 +6599,210 @@
         <v>1994</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>15</v>
+        <v>189</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F302" s="3" t="s">
+        <v>356</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H302" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A303" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F303" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F304" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F305" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F306" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F307" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B303" s="2" t="s">
+      <c r="B308" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C303" s="1">
+      <c r="C308" s="1">
         <v>1994</v>
-      </c>
-      <c r="D303" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G303" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H303" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A304" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B304" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C304" s="1">
-        <v>1994</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G304" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H304" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A305" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B305" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C305" s="1">
-        <v>1994</v>
-      </c>
-      <c r="D305" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G305" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H305" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A306" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C306" s="1">
-        <v>1994</v>
-      </c>
-      <c r="D306" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G306" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H306" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A307" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B307" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C307" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F307" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="G307" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H307" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A308" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B308" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C308" s="1">
-        <v>1995</v>
       </c>
       <c r="D308" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E308" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="G308" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H308" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C309" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H309" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C310" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="F310" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H310" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C311" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>358</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H311" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C312" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
+      </c>
+      <c r="E312" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="G312" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H312" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A313" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B313" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C313" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D313" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G313" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H313" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A314" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C314" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D314" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G314" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H314" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A315" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B315" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C315" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G315" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H315" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A316" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C316" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D316" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G316" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H316" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A317" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B317" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C317" s="1">
-        <v>1995</v>
-      </c>
-      <c r="D317" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G317" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H317" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F313" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F314" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F315" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F316" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F317" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C318" s="1">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>31</v>
+        <v>132</v>
+      </c>
+      <c r="E318" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F318" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="G318" s="1" t="s">
         <v>16</v>
@@ -6812,307 +6811,286 @@
         <v>72</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A319" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C319" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D319" s="1" t="s">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F319" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F320" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F321" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C322" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E322" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F322" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G322" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H322" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C323" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F323" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G323" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H323" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F324" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C325" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E325" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F325" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G325" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H325" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C326" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F326" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G326" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H326" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A327" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C327" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F327" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G327" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H327" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A328" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C328" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F328" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="G328" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H328" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A329" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C329" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G329" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H329" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A330" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C330" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D330" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G319" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H319" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A320" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B320" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C320" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D320" s="1" t="s">
+      <c r="E330" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F330" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H330" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A331" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C331" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D331" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G320" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H320" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A321" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C321" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D321" s="1" t="s">
+      <c r="F331" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="G331" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A332" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C332" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D332" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G321" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H321" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A322" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B322" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C322" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D322" s="1" t="s">
+      <c r="F332" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G332" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H332" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A333" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C333" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D333" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G322" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H322" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A323" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B323" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C323" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D323" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G323" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H323" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A324" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C324" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D324" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G324" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H324" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A325" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B325" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C325" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D325" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G325" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H325" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A326" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B326" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C326" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D326" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G326" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H326" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A327" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B327" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C327" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D327" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G327" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H327" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A328" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B328" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C328" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D328" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G328" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H328" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A329" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B329" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C329" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D329" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G329" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H329" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A330" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B330" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C330" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D330" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G330" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H330" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A331" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B331" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C331" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D331" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G331" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H331" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A332" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B332" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C332" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D332" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G332" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H332" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A333" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C333" s="1">
-        <v>1996</v>
-      </c>
-      <c r="D333" s="1" t="s">
-        <v>201</v>
+      <c r="F333" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H333" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>191</v>
       </c>
@@ -7123,16 +7101,22 @@
         <v>1996</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="E334" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F334" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H334" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>191</v>
       </c>
@@ -7143,16 +7127,19 @@
         <v>1996</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="F335" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="G335" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H335" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>191</v>
       </c>
@@ -7163,16 +7150,19 @@
         <v>1996</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="F336" s="3" t="s">
+        <v>365</v>
       </c>
       <c r="G336" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H336" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>191</v>
       </c>
@@ -7183,16 +7173,19 @@
         <v>1996</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="F337" s="3" t="s">
+        <v>366</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H337" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>191</v>
       </c>
@@ -7203,16 +7196,16 @@
         <v>1996</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H338" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>191</v>
       </c>
@@ -7223,393 +7216,928 @@
         <v>1996</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H339" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C340" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H340" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C341" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H341" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C342" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H342" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C343" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G343" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H343" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C344" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G344" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H344" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C345" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>15</v>
+        <v>118</v>
+      </c>
+      <c r="E345" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F345" s="3" t="s">
+        <v>367</v>
       </c>
       <c r="G345" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H345" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C346" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
+      </c>
+      <c r="F346" s="3" t="s">
+        <v>368</v>
       </c>
       <c r="G346" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H346" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C347" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>15</v>
+        <v>118</v>
+      </c>
+      <c r="F347" s="3" t="s">
+        <v>331</v>
       </c>
       <c r="G347" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H347" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A348" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B348" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C348" s="1">
-        <v>1998</v>
-      </c>
-      <c r="D348" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G348" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H348" s="1" t="s">
-        <v>134</v>
+      <c r="F348" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C349" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>15</v>
+        <v>201</v>
+      </c>
+      <c r="E349" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F349" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="G349" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H349" s="1" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C350" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>163</v>
+        <v>201</v>
+      </c>
+      <c r="F350" s="3" t="s">
+        <v>360</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H350" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C351" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>163</v>
+        <v>201</v>
+      </c>
+      <c r="F351" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H351" s="1" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="C352" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>163</v>
+        <v>201</v>
+      </c>
+      <c r="F352" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H352" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C353" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="G353" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H353" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C354" s="1">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H354" s="1" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C355" s="1">
-        <v>2000</v>
+        <v>1996</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="G355" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H355" s="1" t="s">
-        <v>18</v>
+        <v>203</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C356" s="1">
-        <v>2000</v>
+        <v>1996</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H356" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C357" s="1">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
+      </c>
+      <c r="E357" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F357" s="3" t="s">
+        <v>328</v>
       </c>
       <c r="G357" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H357" s="1" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C358" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F358" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G358" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H358" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F359" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F360" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F361" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A362" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B362" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C362" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F362" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A363" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B363" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C363" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F363" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A364" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C364" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A365" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C365" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F365" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G365" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A366" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C366" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E366" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F366" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="G366" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H366" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F367" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F368" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F369" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A370" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C370" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E370" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F370" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A371" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C371" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A372" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C372" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F372" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C373" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E373" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F373" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A374" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C374" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F374" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A375" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C375" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F375" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A376" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C376" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E376" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F376" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F377" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F378" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F379" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F380" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F381" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C382" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E382" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F382" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F383" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F384" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F385" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A386" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B358" s="2" t="s">
+      <c r="B386" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C358" s="1">
+      <c r="C386" s="1">
         <v>2000</v>
       </c>
-      <c r="D358" s="1" t="s">
+      <c r="D386" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E386" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F386" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A387" s="3"/>
+      <c r="F387" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A388" s="3"/>
+      <c r="F388" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A389" s="3"/>
+      <c r="F389" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A390" s="3"/>
+      <c r="F390" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C391" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D391" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G358" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H358" s="1" t="s">
+      <c r="E391" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F391" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C392" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F392" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C393" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F393" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H393" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F394" s="3" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>